<commit_message>
Añadido el tiempo de estudio para examenes
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Calendario-Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E10420-9522-4E69-85C4-1B0BACCAD59F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E2C358F-8A7E-49C5-AF48-4409E99AECAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E527D347-6773-4830-B6E6-2B05EAFEE885}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{E527D347-6773-4830-B6E6-2B05EAFEE885}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="14">
   <si>
     <t>FEBRERO</t>
   </si>
@@ -76,6 +76,9 @@
   <si>
     <t>Carlos Andrés Mesa Roldan (CC 1044508253)</t>
   </si>
+  <si>
+    <t>TrabajoExtra</t>
+  </si>
 </sst>
 </file>
 
@@ -90,7 +93,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,6 +154,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -197,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -241,6 +250,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85BD0A8B-7FCE-440A-980B-F116DB20E08C}">
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,8 +880,8 @@
       <c r="F8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>10</v>
+      <c r="G8" s="17" t="s">
+        <v>13</v>
       </c>
       <c r="I8" s="3">
         <v>0.66666666666666663</v>
@@ -914,8 +924,8 @@
       <c r="F9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>10</v>
+      <c r="G9" s="17" t="s">
+        <v>13</v>
       </c>
       <c r="I9" s="3">
         <v>0.75</v>
@@ -1578,6 +1588,11 @@
         <v>10</v>
       </c>
     </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="D1:E1"/>

</xml_diff>

<commit_message>
Añadido tiempo para estudio de próximos parciales
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Calendario-Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E2C358F-8A7E-49C5-AF48-4409E99AECAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1883B9-A1A6-424A-BC48-17B443968784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{E527D347-6773-4830-B6E6-2B05EAFEE885}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="15">
   <si>
     <t>FEBRERO</t>
   </si>
@@ -79,6 +79,9 @@
   <si>
     <t>TrabajoExtra</t>
   </si>
+  <si>
+    <t>EstudioParcial</t>
+  </si>
 </sst>
 </file>
 
@@ -93,7 +96,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -160,6 +163,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -206,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -251,6 +260,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,7 +578,7 @@
   <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,8 +714,8 @@
       <c r="F4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>10</v>
+      <c r="G4" s="18" t="s">
+        <v>14</v>
       </c>
       <c r="I4" s="3">
         <v>0.33333333333333331</v>
@@ -748,8 +758,8 @@
       <c r="F5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>10</v>
+      <c r="G5" s="18" t="s">
+        <v>14</v>
       </c>
       <c r="I5" s="3">
         <v>0.41666666666666669</v>
@@ -1051,8 +1061,8 @@
       <c r="A13" s="3">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>10</v>
+      <c r="B13" s="18" t="s">
+        <v>14</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>3</v>
@@ -1095,8 +1105,8 @@
       <c r="A14" s="3">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>10</v>
+      <c r="B14" s="18" t="s">
+        <v>14</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>9</v>
@@ -1227,8 +1237,8 @@
       <c r="A17" s="3">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>10</v>
+      <c r="B17" s="17" t="s">
+        <v>13</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>4</v>
@@ -1271,8 +1281,8 @@
       <c r="A18" s="3">
         <v>0.75</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>10</v>
+      <c r="B18" s="17" t="s">
+        <v>13</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>11</v>
@@ -1592,6 +1602,9 @@
       <c r="A32" s="17" t="s">
         <v>13</v>
       </c>
+      <c r="B32" s="18" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Confirmadas algunas fechas de parciales
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Calendario-Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1883B9-A1A6-424A-BC48-17B443968784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4D8898-D19E-4684-9E9A-671C517B2694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{E527D347-6773-4830-B6E6-2B05EAFEE885}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E527D347-6773-4830-B6E6-2B05EAFEE885}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="17">
   <si>
     <t>FEBRERO</t>
   </si>
@@ -82,6 +82,12 @@
   <si>
     <t>EstudioParcial</t>
   </si>
+  <si>
+    <t>Parciales</t>
+  </si>
+  <si>
+    <t>Parcial</t>
+  </si>
 </sst>
 </file>
 
@@ -96,7 +102,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,6 +175,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -215,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -247,6 +259,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -259,8 +273,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,7 +594,7 @@
   <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,22 +610,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="14" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="13" t="s">
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="13"/>
+      <c r="M1" s="15"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -714,7 +730,7 @@
       <c r="F4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="14" t="s">
         <v>14</v>
       </c>
       <c r="I4" s="3">
@@ -758,7 +774,7 @@
       <c r="F5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="14" t="s">
         <v>14</v>
       </c>
       <c r="I5" s="3">
@@ -811,8 +827,8 @@
       <c r="J6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K6" s="11" t="s">
-        <v>9</v>
+      <c r="K6" s="20" t="s">
+        <v>16</v>
       </c>
       <c r="L6" s="7" t="s">
         <v>3</v>
@@ -890,7 +906,7 @@
       <c r="F8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="13" t="s">
         <v>13</v>
       </c>
       <c r="I8" s="3">
@@ -934,7 +950,7 @@
       <c r="F9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="13" t="s">
         <v>13</v>
       </c>
       <c r="I9" s="3">
@@ -1061,7 +1077,7 @@
       <c r="A13" s="3">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -1105,7 +1121,7 @@
       <c r="A14" s="3">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="11" t="s">
@@ -1237,7 +1253,7 @@
       <c r="A17" s="3">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -1264,8 +1280,8 @@
       <c r="K17" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="L17" s="8" t="s">
-        <v>4</v>
+      <c r="L17" s="20" t="s">
+        <v>16</v>
       </c>
       <c r="M17" s="10" t="s">
         <v>7</v>
@@ -1281,7 +1297,7 @@
       <c r="A18" s="3">
         <v>0.75</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="12" t="s">
@@ -1464,8 +1480,8 @@
       <c r="D24" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="11" t="s">
-        <v>9</v>
+      <c r="E24" s="14" t="s">
+        <v>14</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -1494,8 +1510,8 @@
       <c r="D25" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="11" t="s">
-        <v>9</v>
+      <c r="E25" s="14" t="s">
+        <v>14</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -1599,11 +1615,14 @@
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="14" t="s">
         <v>14</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Añadido tiempo estudiar en examenes
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Calendario-Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4D8898-D19E-4684-9E9A-671C517B2694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAFF946-F0AA-41D2-B66F-EE3C7605D23A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E527D347-6773-4830-B6E6-2B05EAFEE885}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{E527D347-6773-4830-B6E6-2B05EAFEE885}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -261,6 +261,10 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -271,10 +275,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -593,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85BD0A8B-7FCE-440A-980B-F116DB20E08C}">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,22 +610,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="16" t="s">
+      <c r="E1" s="17"/>
+      <c r="F1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="15" t="s">
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="15"/>
+      <c r="M1" s="17"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -745,8 +745,8 @@
       <c r="L4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="M4" s="2" t="s">
-        <v>10</v>
+      <c r="M4" s="12" t="s">
+        <v>11</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>10</v>
@@ -789,8 +789,8 @@
       <c r="L5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="2" t="s">
-        <v>10</v>
+      <c r="M5" s="12" t="s">
+        <v>11</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>10</v>
@@ -827,14 +827,14 @@
       <c r="J6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K6" s="20" t="s">
+      <c r="K6" s="16" t="s">
         <v>16</v>
       </c>
       <c r="L6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="M6" s="2" t="s">
-        <v>10</v>
+      <c r="M6" s="12" t="s">
+        <v>11</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>10</v>
@@ -877,8 +877,8 @@
       <c r="L7" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="2" t="s">
-        <v>10</v>
+      <c r="M7" s="12" t="s">
+        <v>11</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>10</v>
@@ -921,8 +921,8 @@
       <c r="L8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="M8" s="2" t="s">
-        <v>10</v>
+      <c r="M8" s="12" t="s">
+        <v>11</v>
       </c>
       <c r="N8" s="2" t="s">
         <v>10</v>
@@ -965,8 +965,8 @@
       <c r="L9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="M9" s="2" t="s">
-        <v>10</v>
+      <c r="M9" s="12" t="s">
+        <v>11</v>
       </c>
       <c r="N9" s="2" t="s">
         <v>10</v>
@@ -1280,7 +1280,7 @@
       <c r="K17" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="L17" s="20" t="s">
+      <c r="L17" s="16" t="s">
         <v>16</v>
       </c>
       <c r="M17" s="10" t="s">
@@ -1621,7 +1621,7 @@
       <c r="B32" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="19" t="s">
+      <c r="C32" s="15" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se actualizaron fechas de trabajo y días para próximas evaluaciones
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Calendario-Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAFF946-F0AA-41D2-B66F-EE3C7605D23A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4103EB9D-D0FF-4982-84FE-DB794C0C6676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{E527D347-6773-4830-B6E6-2B05EAFEE885}"/>
   </bookViews>
@@ -593,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85BD0A8B-7FCE-440A-980B-F116DB20E08C}">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1110,8 +1110,8 @@
       <c r="M13" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="N13" s="2" t="s">
-        <v>10</v>
+      <c r="N13" s="12" t="s">
+        <v>11</v>
       </c>
       <c r="O13" s="2" t="s">
         <v>10</v>
@@ -1151,11 +1151,11 @@
       <c r="L14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="M14" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>10</v>
+      <c r="M14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N14" s="12" t="s">
+        <v>11</v>
       </c>
       <c r="O14" s="2" t="s">
         <v>10</v>
@@ -1198,8 +1198,8 @@
       <c r="M15" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="N15" s="2" t="s">
-        <v>10</v>
+      <c r="N15" s="12" t="s">
+        <v>11</v>
       </c>
       <c r="O15" s="2" t="s">
         <v>10</v>
@@ -1239,14 +1239,14 @@
       <c r="L16" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="M16" s="11" t="s">
-        <v>9</v>
+      <c r="M16" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="O16" s="2" t="s">
-        <v>10</v>
+      <c r="O16" s="12" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -1327,8 +1327,8 @@
       <c r="L18" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="M18" s="11" t="s">
-        <v>9</v>
+      <c r="M18" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="N18" s="2" t="s">
         <v>10</v>

</xml_diff>